<commit_message>
Link Repo & names
</commit_message>
<xml_diff>
--- a/Security Task Team Information.xlsx
+++ b/Security Task Team Information.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2602751D-A614-2B46-AE88-DC3B92C3B2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makka\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D07611-060B-4F02-845B-507462F4CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>لينك ال repo</t>
   </si>
@@ -51,14 +56,32 @@
     <t>اسم الفرد السادس</t>
   </si>
   <si>
-    <t>اسم الفرد السابع</t>
+    <t xml:space="preserve">احمد خالد محمد </t>
+  </si>
+  <si>
+    <t>إسماعيل عبدالله عزب</t>
+  </si>
+  <si>
+    <t>حنان احمد مصطفي</t>
+  </si>
+  <si>
+    <t>روان زينهم عبدالعزيز</t>
+  </si>
+  <si>
+    <t>عبدالله محمد خالد عبدالباسط</t>
+  </si>
+  <si>
+    <t>عبدالرحمن علاء الدين عبدالمنعم</t>
+  </si>
+  <si>
+    <t>https://github.com/AbdallahHikal/Steganography.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -74,6 +97,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -101,15 +131,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -326,16 +364,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="C9:F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.67578125" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="2" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -357,11 +402,35 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{03467FED-0208-4A25-A788-A9E8AD3C9445}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>